<commit_message>
small corrections to some questions
</commit_message>
<xml_diff>
--- a/devset/Legal questions Adam.xlsx
+++ b/devset/Legal questions Adam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamwagnerhoegh/Documents/SODAS/sem3/nlp_itu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F2AECE-0CDF-B74A-82A4-2BD7A90EA259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B62462-8D8D-C142-A8EE-17F87C6B4FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17220" xr2:uid="{55C6936D-CA1B-3E49-80A2-0F9F885B54C9}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>LBK nr 978 af 19/10/2009'</t>
   </si>
   <si>
-    <t>Hvem kan på baggrund af en evaluering fastsætte regler om kvalitetsudvikling, herunder lærerkvalifikationer mv.</t>
-  </si>
-  <si>
     <t>Undervisningsministeren kan  på baggrund af en evaluering fastsætte regler om kvalitetsudvikling, herunder lærerkvalifikationer m.v.</t>
   </si>
   <si>
@@ -507,6 +504,9 @@
   </si>
   <si>
     <t>LOV nr 473 af 12/06/2009</t>
+  </si>
+  <si>
+    <t>Hvem kan på baggrund af en evaluering fastsætte regler om kvalitetsudvikling, herunder lærerkvalifikationer mv?</t>
   </si>
 </sst>
 </file>
@@ -917,7 +917,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,7 +981,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -1049,242 +1049,242 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" t="s">
         <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D10">
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
         <v>41</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
       </c>
       <c r="D11">
         <v>813</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D14">
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
       </c>
       <c r="D16">
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D17">
         <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" t="s">
         <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
         <v>78</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>79</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D21">
         <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" t="s">
         <v>88</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -1292,290 +1292,290 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="D24" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>97</v>
-      </c>
-      <c r="E24" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D25">
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
         <v>102</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" t="s">
         <v>103</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" t="s">
         <v>106</v>
-      </c>
-      <c r="C27" t="s">
-        <v>107</v>
       </c>
       <c r="D27">
         <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D28">
         <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D29">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
         <v>115</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D30">
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D31">
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" t="s">
         <v>124</v>
-      </c>
-      <c r="C32" t="s">
-        <v>125</v>
       </c>
       <c r="D32">
         <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" t="s">
         <v>128</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>129</v>
       </c>
-      <c r="D33" t="s">
-        <v>130</v>
-      </c>
       <c r="E33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" t="s">
         <v>132</v>
-      </c>
-      <c r="C34" t="s">
-        <v>133</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
         <v>135</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>136</v>
-      </c>
-      <c r="C35" t="s">
-        <v>137</v>
       </c>
       <c r="D35">
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" t="s">
         <v>140</v>
-      </c>
-      <c r="C36" t="s">
-        <v>141</v>
       </c>
       <c r="D36">
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" t="s">
         <v>146</v>
-      </c>
-      <c r="C38" t="s">
-        <v>147</v>
       </c>
       <c r="D38">
         <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" t="s">
         <v>149</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>150</v>
-      </c>
-      <c r="C39" t="s">
-        <v>151</v>
       </c>
       <c r="D39">
         <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" t="s">
         <v>153</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>154</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>155</v>
-      </c>
-      <c r="E40" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>